<commit_message>
Chart and Output excel file Done!!
</commit_message>
<xml_diff>
--- a/scheduleData.xlsx
+++ b/scheduleData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>09:00</t>
   </si>
@@ -23,16 +23,16 @@
     <t>08:30</t>
   </si>
   <si>
-    <t>11:30</t>
+    <t>09:25</t>
   </si>
   <si>
     <t>10:00</t>
   </si>
   <si>
-    <t>10:28</t>
-  </si>
-  <si>
-    <t>09:26</t>
+    <t>11:35</t>
+  </si>
+  <si>
+    <t>09:49</t>
   </si>
   <si>
     <t>14:00</t>
@@ -41,16 +41,22 @@
     <t>14:18</t>
   </si>
   <si>
+    <t>11:00</t>
+  </si>
+  <si>
+    <t>12:15</t>
+  </si>
+  <si>
     <t>10:18</t>
   </si>
   <si>
     <t>14:50</t>
   </si>
   <si>
-    <t>11:00</t>
-  </si>
-  <si>
     <t>11:21</t>
+  </si>
+  <si>
+    <t>10:26</t>
   </si>
 </sst>
 </file>
@@ -95,7 +101,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -129,7 +135,7 @@
         <v>3</v>
       </c>
       <c r="D2" t="n">
-        <v>180.0</v>
+        <v>55.0</v>
       </c>
       <c r="E2" t="n">
         <v>1.0</v>
@@ -146,10 +152,10 @@
         <v>5</v>
       </c>
       <c r="D3" t="n">
-        <v>28.0</v>
+        <v>95.0</v>
       </c>
       <c r="E3" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="4">
@@ -163,10 +169,10 @@
         <v>6</v>
       </c>
       <c r="D4" t="n">
-        <v>26.0</v>
+        <v>49.0</v>
       </c>
       <c r="E4" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="5">
@@ -188,53 +194,87 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6" t="n">
-        <v>18.0</v>
+        <v>75.0</v>
       </c>
       <c r="E6" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>10.0</v>
+        <v>7.0</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D7" t="n">
-        <v>50.0</v>
+        <v>18.0</v>
       </c>
       <c r="E7" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
       </c>
       <c r="D8" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="n">
         <v>21.0</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E9" t="n">
         <v>3.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>7.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final reservation done for S_C,C_C_S,Chademo.
</commit_message>
<xml_diff>
--- a/scheduleData.xlsx
+++ b/scheduleData.xlsx
@@ -12,51 +12,75 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+  <si>
+    <t>08:30</t>
+  </si>
+  <si>
+    <t>08:34</t>
+  </si>
+  <si>
+    <t>09:30</t>
+  </si>
+  <si>
+    <t>09:43</t>
+  </si>
+  <si>
+    <t>11:00</t>
+  </si>
+  <si>
+    <t>11:13</t>
+  </si>
+  <si>
+    <t>11:14</t>
+  </si>
+  <si>
+    <t>11:18</t>
+  </si>
+  <si>
+    <t>14:00</t>
+  </si>
+  <si>
+    <t>14:18</t>
+  </si>
+  <si>
+    <t>14:19</t>
+  </si>
+  <si>
+    <t>14:28</t>
+  </si>
   <si>
     <t>09:00</t>
   </si>
   <si>
+    <t>09:26</t>
+  </si>
+  <si>
+    <t>10:00</t>
+  </si>
+  <si>
+    <t>10:26</t>
+  </si>
+  <si>
+    <t>10:18</t>
+  </si>
+  <si>
+    <t>10:27</t>
+  </si>
+  <si>
+    <t>10:41</t>
+  </si>
+  <si>
+    <t>11:11</t>
+  </si>
+  <si>
+    <t>10:05</t>
+  </si>
+  <si>
     <t>10:06</t>
   </si>
   <si>
-    <t>08:30</t>
-  </si>
-  <si>
-    <t>09:25</t>
-  </si>
-  <si>
-    <t>10:00</t>
-  </si>
-  <si>
-    <t>11:35</t>
-  </si>
-  <si>
-    <t>09:49</t>
-  </si>
-  <si>
-    <t>14:00</t>
-  </si>
-  <si>
-    <t>14:18</t>
-  </si>
-  <si>
-    <t>11:00</t>
-  </si>
-  <si>
-    <t>12:15</t>
-  </si>
-  <si>
-    <t>10:18</t>
-  </si>
-  <si>
-    <t>14:50</t>
-  </si>
-  <si>
-    <t>11:21</t>
-  </si>
-  <si>
-    <t>10:26</t>
+    <t>10:14</t>
   </si>
 </sst>
 </file>
@@ -101,7 +125,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -109,7 +133,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -118,15 +142,15 @@
         <v>1</v>
       </c>
       <c r="D1" t="n">
-        <v>66.0</v>
+        <v>4.0</v>
       </c>
       <c r="E1" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2.0</v>
+        <v>13.0</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -135,15 +159,15 @@
         <v>3</v>
       </c>
       <c r="D2" t="n">
-        <v>55.0</v>
+        <v>13.0</v>
       </c>
       <c r="E2" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -152,27 +176,27 @@
         <v>5</v>
       </c>
       <c r="D3" t="n">
-        <v>95.0</v>
+        <v>13.0</v>
       </c>
       <c r="E3" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="n">
         <v>4.0</v>
       </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="n">
-        <v>49.0</v>
-      </c>
       <c r="E4" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="5">
@@ -180,10 +204,10 @@
         <v>5.0</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5" t="n">
         <v>18.0</v>
@@ -194,33 +218,33 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>6.0</v>
+        <v>10.0</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6" t="n">
-        <v>75.0</v>
+        <v>9.0</v>
       </c>
       <c r="E6" t="n">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>7.0</v>
+        <v>4.0</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D7" t="n">
-        <v>18.0</v>
+        <v>26.0</v>
       </c>
       <c r="E7" t="n">
         <v>2.0</v>
@@ -228,53 +252,104 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>10.0</v>
+        <v>12.0</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D8" t="n">
-        <v>50.0</v>
+        <v>26.0</v>
       </c>
       <c r="E8" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>11.0</v>
+        <v>7.0</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D9" t="n">
-        <v>21.0</v>
+        <v>18.0</v>
       </c>
       <c r="E9" t="n">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>12.0</v>
+        <v>3.0</v>
       </c>
       <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B11" t="s">
         <v>4</v>
       </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" t="n">
-        <v>26.0</v>
-      </c>
-      <c r="E10" t="n">
-        <v>7.0</v>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="n">
+        <v>65.0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>3.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactoring And Optimization in progress Done!!
</commit_message>
<xml_diff>
--- a/scheduleData.xlsx
+++ b/scheduleData.xlsx
@@ -12,7 +12,46 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+  <si>
+    <t>09:00</t>
+  </si>
+  <si>
+    <t>09:26</t>
+  </si>
+  <si>
+    <t>09:27</t>
+  </si>
+  <si>
+    <t>09:32</t>
+  </si>
+  <si>
+    <t>09:33</t>
+  </si>
+  <si>
+    <t>09:38</t>
+  </si>
+  <si>
+    <t>10:00</t>
+  </si>
+  <si>
+    <t>10:26</t>
+  </si>
+  <si>
+    <t>10:27</t>
+  </si>
+  <si>
+    <t>10:41</t>
+  </si>
+  <si>
+    <t>11:00</t>
+  </si>
+  <si>
+    <t>11:11</t>
+  </si>
+  <si>
+    <t>10:18</t>
+  </si>
   <si>
     <t>08:30</t>
   </si>
@@ -26,9 +65,6 @@
     <t>09:43</t>
   </si>
   <si>
-    <t>11:00</t>
-  </si>
-  <si>
     <t>11:13</t>
   </si>
   <si>
@@ -48,30 +84,6 @@
   </si>
   <si>
     <t>14:28</t>
-  </si>
-  <si>
-    <t>09:00</t>
-  </si>
-  <si>
-    <t>09:26</t>
-  </si>
-  <si>
-    <t>10:00</t>
-  </si>
-  <si>
-    <t>10:26</t>
-  </si>
-  <si>
-    <t>10:18</t>
-  </si>
-  <si>
-    <t>10:27</t>
-  </si>
-  <si>
-    <t>10:41</t>
-  </si>
-  <si>
-    <t>11:11</t>
   </si>
   <si>
     <t>10:05</t>
@@ -125,7 +137,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -133,7 +145,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -142,15 +154,15 @@
         <v>1</v>
       </c>
       <c r="D1" t="n">
-        <v>4.0</v>
+        <v>26.0</v>
       </c>
       <c r="E1" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>13.0</v>
+        <v>17.0</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -159,15 +171,15 @@
         <v>3</v>
       </c>
       <c r="D2" t="n">
-        <v>13.0</v>
+        <v>5.0</v>
       </c>
       <c r="E2" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>6.0</v>
+        <v>18.0</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -176,15 +188,15 @@
         <v>5</v>
       </c>
       <c r="D3" t="n">
-        <v>13.0</v>
+        <v>5.0</v>
       </c>
       <c r="E3" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>9.0</v>
+        <v>12.0</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -193,15 +205,15 @@
         <v>7</v>
       </c>
       <c r="D4" t="n">
-        <v>4.0</v>
+        <v>26.0</v>
       </c>
       <c r="E4" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -210,15 +222,15 @@
         <v>9</v>
       </c>
       <c r="D5" t="n">
-        <v>18.0</v>
+        <v>14.0</v>
       </c>
       <c r="E5" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -227,128 +239,162 @@
         <v>11</v>
       </c>
       <c r="D6" t="n">
-        <v>9.0</v>
+        <v>11.0</v>
       </c>
       <c r="E6" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>4.0</v>
+        <v>7.0</v>
       </c>
       <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
       <c r="D7" t="n">
-        <v>26.0</v>
+        <v>18.0</v>
       </c>
       <c r="E7" t="n">
-        <v>2.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>12.0</v>
+        <v>2.0</v>
       </c>
       <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
         <v>14</v>
       </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
       <c r="D8" t="n">
-        <v>26.0</v>
+        <v>4.0</v>
       </c>
       <c r="E8" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>7.0</v>
+        <v>13.0</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
         <v>16</v>
       </c>
       <c r="D9" t="n">
-        <v>18.0</v>
+        <v>13.0</v>
       </c>
       <c r="E9" t="n">
-        <v>7.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
         <v>17</v>
       </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
       <c r="D10" t="n">
-        <v>14.0</v>
+        <v>13.0</v>
       </c>
       <c r="E10" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>11.0</v>
+        <v>9.0</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
         <v>19</v>
       </c>
       <c r="D11" t="n">
-        <v>11.0</v>
+        <v>4.0</v>
       </c>
       <c r="E11" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D12" t="n">
-        <v>65.0</v>
+        <v>18.0</v>
       </c>
       <c r="E12" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="n">
+        <v>65.0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
         <v>14.0</v>
       </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" t="n">
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" t="n">
         <v>8.0</v>
       </c>
-      <c r="E13" t="n">
+      <c r="E15" t="n">
         <v>3.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
little bug fix Optimization Done!!
</commit_message>
<xml_diff>
--- a/scheduleData.xlsx
+++ b/scheduleData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>09:00</t>
   </si>
@@ -92,7 +92,10 @@
     <t>10:06</t>
   </si>
   <si>
-    <t>10:14</t>
+    <t>10:19</t>
+  </si>
+  <si>
+    <t>10:10</t>
   </si>
 </sst>
 </file>
@@ -137,7 +140,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -383,19 +386,53 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>14.0</v>
+        <v>19.0</v>
       </c>
       <c r="B15" t="s">
         <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="D15" t="n">
-        <v>8.0</v>
+        <v>12.0</v>
       </c>
       <c r="E15" t="n">
         <v>3.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>